<commit_message>
fix sort & detail response
</commit_message>
<xml_diff>
--- a/bug_report_10_records.xlsx
+++ b/bug_report_10_records.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cuong\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AIReady_Group4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABAE85BE-0B5C-420A-8335-D5B257176CCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFE7C39-447A-481A-92F5-85312D5E34C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,13 +70,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4472C4"/>
+        <bgColor rgb="FF4472C4"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -91,8 +103,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,9 +412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -407,10 +420,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
support all bug template
</commit_message>
<xml_diff>
--- a/bug_report_10_records.xlsx
+++ b/bug_report_10_records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AIReady_Group4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFE7C39-447A-481A-92F5-85312D5E34C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BBA7B1-7C5C-4BD8-B177-C87FD2C48003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
   <si>
     <t>No</t>
   </si>
   <si>
-    <t>Nội dung bug</t>
-  </si>
-  <si>
     <t>Không đăng nhập được khi sai mật khẩu</t>
   </si>
   <si>
@@ -56,13 +53,159 @@
   </si>
   <si>
     <t>Không tự động reload dữ liệu sau khi cập nhật</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>ScreenId</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Reporter</t>
+  </si>
+  <si>
+    <t>Create date</t>
+  </si>
+  <si>
+    <t>Due date</t>
+  </si>
+  <si>
+    <t>Closed date</t>
+  </si>
+  <si>
+    <t>Assignee</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>SRC_PRODUCT_01</t>
+  </si>
+  <si>
+    <t>SRC_ORDER_03</t>
+  </si>
+  <si>
+    <t>SRC_CUSTOMER_02</t>
+  </si>
+  <si>
+    <t>SRC_PRINT_01</t>
+  </si>
+  <si>
+    <t>SRC_UI_05</t>
+  </si>
+  <si>
+    <t>SRC_SEARCH_01</t>
+  </si>
+  <si>
+    <t>SRC_STOCK_04</t>
+  </si>
+  <si>
+    <t>SRC_ORDER_01</t>
+  </si>
+  <si>
+    <t>SRC_REPORT_02</t>
+  </si>
+  <si>
+    <t>SRC_LOGIN_01</t>
+  </si>
+  <si>
+    <t>TC_LOGIN_003
+Steps: 1) Mở màn hình đăng nhập 2) Nhập tài khoản hợp lệ 3) Nhập mật khẩu sai 4) Nhấn Đăng nhập
+Expected: Hiển thị lỗi sai mật khẩu
+Actual: Không hiển thị lỗi</t>
+  </si>
+  <si>
+    <t>TC_API_015
+Steps: Gửi request payload 5MB
+Expected: Trả về 400 hoặc 413
+Actual: Server trả 500</t>
+  </si>
+  <si>
+    <t>TC_UI_021
+Steps: Mở trang cập nhật sản phẩm → Nhấn Lưu
+Expected: Lưu thành công
+Actual: Không có phản hồi</t>
+  </si>
+  <si>
+    <t>TC_CART_009
+Expected: Tổng = 250.000
+Actual: Hiển thị 200.000</t>
+  </si>
+  <si>
+    <t>TC_UI_033
+Expected: Font chuẩn
+Actual: Font fallback trên mobile</t>
+  </si>
+  <si>
+    <t>TC_UPLOAD_012
+Expected: Upload thành công hoặc báo lỗi
+Actual: UI đứng, không thông báo</t>
+  </si>
+  <si>
+    <t>TC_FORM_004
+Expected: Reset form
+Actual: Dữ liệu vẫn còn</t>
+  </si>
+  <si>
+    <t>TC_WS_003
+Expected: Duy trì hoặc tự reconnect
+Actual: Ngắt kết nối sau 30 giây</t>
+  </si>
+  <si>
+    <t>TC_ERROR_017
+Expected: Hiển thị lỗi timeout
+Actual: UI chờ mãi không báo lỗi</t>
+  </si>
+  <si>
+    <t>TC_REFRESH_006
+Expected: Reload dữ liệu tự động
+Actual: Phải nhấn F5 mới thấy thay đổi</t>
+  </si>
+  <si>
+    <t>Tester1</t>
+  </si>
+  <si>
+    <t>Tester2</t>
+  </si>
+  <si>
+    <t>Tester3</t>
+  </si>
+  <si>
+    <t>Tester4</t>
+  </si>
+  <si>
+    <t>Tester5</t>
+  </si>
+  <si>
+    <t>Tester6</t>
+  </si>
+  <si>
+    <t>Tester7</t>
+  </si>
+  <si>
+    <t>Tester8</t>
+  </si>
+  <si>
+    <t>Tester9</t>
+  </si>
+  <si>
+    <t>Tester10</t>
+  </si>
+  <si>
+    <t>Open</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +218,12 @@
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -103,10 +252,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -410,104 +568,330 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="9" width="19.85546875" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="4">
+        <v>45995</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="4">
+        <v>45995</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="4">
+        <v>45995</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="4">
+        <v>45995</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="4">
+        <v>45995</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="4">
+        <v>45995</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="4">
+        <v>45995</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="4">
+        <v>45995</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="4">
+        <v>45995</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>11</v>
+      <c r="C11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="4">
+        <v>45995</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>